<commit_message>
First set of README tweaks/clarifications
</commit_message>
<xml_diff>
--- a/BerkeleyGW/visualization/results-summary.xlsx
+++ b/BerkeleyGW/visualization/results-summary.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10727"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11122"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jclary/dft/hpcapps/bgw-gpu-benchmarking/combined/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CC6B7CD-C4D0-3043-98A6-71E57E90ADC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A46C6C80-44AB-B14B-94B2-71BA28F7C59F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-6440" yWindow="-17780" windowWidth="28040" windowHeight="17440" xr2:uid="{B298EEBF-4254-C240-989C-A4C0E8CF2884}"/>
   </bookViews>
@@ -41,9 +41,6 @@
     <t>Benchmarker</t>
   </si>
   <si>
-    <t>NREL</t>
-  </si>
-  <si>
     <t>Node Type</t>
   </si>
   <si>
@@ -96,6 +93,9 @@
   </si>
   <si>
     <t>-</t>
+  </si>
+  <si>
+    <t>NLR</t>
   </si>
 </sst>
 </file>
@@ -470,7 +470,7 @@
   <dimension ref="A1:J25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I26" sqref="I26"/>
+      <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -489,45 +489,45 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>8</v>
-      </c>
-      <c r="J1" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>1</v>
+        <v>19</v>
       </c>
       <c r="B2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" t="s">
         <v>10</v>
-      </c>
-      <c r="D2" t="s">
-        <v>11</v>
       </c>
       <c r="E2">
         <v>4</v>
@@ -550,16 +550,16 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>1</v>
+        <v>19</v>
       </c>
       <c r="B3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" t="s">
         <v>10</v>
-      </c>
-      <c r="D3" t="s">
-        <v>11</v>
       </c>
       <c r="E3">
         <v>8</v>
@@ -582,16 +582,16 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>1</v>
+        <v>19</v>
       </c>
       <c r="B4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" t="s">
         <v>10</v>
-      </c>
-      <c r="D4" t="s">
-        <v>11</v>
       </c>
       <c r="E4">
         <v>16</v>
@@ -614,16 +614,16 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>1</v>
+        <v>19</v>
       </c>
       <c r="B5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" t="s">
         <v>10</v>
-      </c>
-      <c r="D5" t="s">
-        <v>11</v>
       </c>
       <c r="E5">
         <v>32</v>
@@ -646,16 +646,16 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>1</v>
+        <v>19</v>
       </c>
       <c r="B6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E6">
         <v>64</v>
@@ -678,16 +678,16 @@
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>1</v>
+        <v>19</v>
       </c>
       <c r="B7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E7">
         <v>96</v>
@@ -710,16 +710,16 @@
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>1</v>
+        <v>19</v>
       </c>
       <c r="B8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E8">
         <v>0.25</v>
@@ -742,16 +742,16 @@
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>1</v>
+        <v>19</v>
       </c>
       <c r="B9" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C9" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E9">
         <v>0.5</v>
@@ -774,16 +774,16 @@
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>1</v>
+        <v>19</v>
       </c>
       <c r="B10" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C10" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D10" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E10">
         <v>1</v>
@@ -806,16 +806,16 @@
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>1</v>
+        <v>19</v>
       </c>
       <c r="B11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C11" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D11" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E11">
         <v>2</v>
@@ -838,16 +838,16 @@
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>1</v>
+        <v>19</v>
       </c>
       <c r="B12" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C12" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D12" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E12">
         <v>4</v>
@@ -870,16 +870,16 @@
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>1</v>
+        <v>19</v>
       </c>
       <c r="B13" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C13" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D13" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E13">
         <v>8</v>
@@ -902,16 +902,16 @@
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>1</v>
+        <v>19</v>
       </c>
       <c r="B14" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C14" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D14" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E14">
         <v>16</v>
@@ -934,16 +934,16 @@
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>1</v>
+        <v>19</v>
       </c>
       <c r="B15" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C15" t="s">
+        <v>11</v>
+      </c>
+      <c r="D15" t="s">
         <v>12</v>
-      </c>
-      <c r="D15" t="s">
-        <v>13</v>
       </c>
       <c r="E15">
         <v>2</v>
@@ -966,16 +966,16 @@
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>1</v>
+        <v>19</v>
       </c>
       <c r="B16" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C16" t="s">
+        <v>11</v>
+      </c>
+      <c r="D16" t="s">
         <v>12</v>
-      </c>
-      <c r="D16" t="s">
-        <v>13</v>
       </c>
       <c r="E16">
         <v>4</v>
@@ -998,16 +998,16 @@
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>1</v>
+        <v>19</v>
       </c>
       <c r="B17" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C17" t="s">
+        <v>11</v>
+      </c>
+      <c r="D17" t="s">
         <v>12</v>
-      </c>
-      <c r="D17" t="s">
-        <v>13</v>
       </c>
       <c r="E17">
         <v>8</v>
@@ -1030,16 +1030,16 @@
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>1</v>
+        <v>19</v>
       </c>
       <c r="B18" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C18" t="s">
+        <v>11</v>
+      </c>
+      <c r="D18" t="s">
         <v>12</v>
-      </c>
-      <c r="D18" t="s">
-        <v>13</v>
       </c>
       <c r="E18">
         <v>16</v>
@@ -1062,16 +1062,16 @@
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>1</v>
+        <v>19</v>
       </c>
       <c r="B19" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C19" t="s">
+        <v>11</v>
+      </c>
+      <c r="D19" t="s">
         <v>12</v>
-      </c>
-      <c r="D19" t="s">
-        <v>13</v>
       </c>
       <c r="E19">
         <v>32</v>
@@ -1094,16 +1094,16 @@
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>1</v>
+        <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C20" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D20" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E20">
         <v>48</v>
@@ -1126,16 +1126,16 @@
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>1</v>
+        <v>19</v>
       </c>
       <c r="B21" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C21" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D21" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E21">
         <v>64</v>
@@ -1158,16 +1158,16 @@
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>1</v>
+        <v>19</v>
       </c>
       <c r="B22" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C22" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D22" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E22">
         <v>96</v>
@@ -1190,98 +1190,98 @@
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
+        <v>17</v>
+      </c>
+      <c r="B23" t="s">
+        <v>16</v>
+      </c>
+      <c r="C23" t="s">
         <v>18</v>
       </c>
-      <c r="B23" t="s">
-        <v>17</v>
-      </c>
-      <c r="C23" t="s">
-        <v>19</v>
-      </c>
       <c r="D23" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E23">
-        <v>24</v>
+        <v>2</v>
       </c>
       <c r="F23" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G23" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H23">
-        <v>305</v>
+        <v>300</v>
       </c>
       <c r="I23">
         <v>5</v>
       </c>
       <c r="J23">
-        <v>300</v>
+        <v>305</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
+        <v>17</v>
+      </c>
+      <c r="B24" t="s">
+        <v>16</v>
+      </c>
+      <c r="C24" t="s">
         <v>18</v>
       </c>
-      <c r="B24" t="s">
-        <v>17</v>
-      </c>
-      <c r="C24" t="s">
-        <v>19</v>
-      </c>
       <c r="D24" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E24">
-        <v>36</v>
+        <v>4</v>
       </c>
       <c r="F24" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G24" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H24">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="I24">
         <v>5</v>
       </c>
       <c r="J24">
-        <v>200</v>
+        <v>205</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
+        <v>17</v>
+      </c>
+      <c r="B25" t="s">
+        <v>16</v>
+      </c>
+      <c r="C25" t="s">
         <v>18</v>
       </c>
-      <c r="B25" t="s">
-        <v>17</v>
-      </c>
-      <c r="C25" t="s">
-        <v>19</v>
-      </c>
       <c r="D25" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E25">
-        <v>48</v>
+        <v>8</v>
       </c>
       <c r="F25" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G25" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H25">
-        <v>155</v>
+        <v>100</v>
       </c>
       <c r="I25">
         <v>5</v>
       </c>
       <c r="J25">
-        <v>150</v>
+        <v>105</v>
       </c>
     </row>
   </sheetData>

</xml_diff>